<commit_message>
Finished EEMs prep for Alan
I finished gathering all of the files for EEMs. I started working on code for the chemical analyses like cond and O2. The code will calculate TDS and work out dilutions/unit conversion.
</commit_message>
<xml_diff>
--- a/1-data/TMP_FEOM_TOC/OneDrive_1_3-21-2024/20240307_Readme_TMP_FEOM_CO_1.xlsx
+++ b/1-data/TMP_FEOM_TOC/OneDrive_1_3-21-2024/20240307_Readme_TMP_FEOM_CO_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olou646\tempest-exp-feom-ConnorSULI\1-data\TMP_FEOM_TOC\OneDrive_1_3-21-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B42772-038C-4121-86CC-37A3160FC4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFAED2F-4204-4894-8BD5-B3482E14BDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FB0433CF-543D-4FDA-A33B-D7DF0F122BC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="159">
   <si>
     <t>Sample Name</t>
   </si>
@@ -507,6 +507,12 @@
   </si>
   <si>
     <t>Dilution correction</t>
+  </si>
+  <si>
+    <t>Omit</t>
+  </si>
+  <si>
+    <t>AW3.01.C</t>
   </si>
 </sst>
 </file>
@@ -882,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280C1DDF-EA1C-4744-B8A7-879B45D19C4D}">
-  <dimension ref="A1:M123"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1158,6 +1164,9 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="C25" t="s">
+        <v>157</v>
+      </c>
       <c r="F25" t="s">
         <v>155</v>
       </c>
@@ -1171,6 +1180,9 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="C26" t="s">
+        <v>157</v>
+      </c>
       <c r="F26" t="s">
         <v>155</v>
       </c>
@@ -1184,6 +1196,9 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
       <c r="F27" t="s">
         <v>155</v>
       </c>
@@ -1197,6 +1212,9 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
       <c r="F28" t="s">
         <v>155</v>
       </c>
@@ -1210,6 +1228,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
+      <c r="C29" t="s">
+        <v>157</v>
+      </c>
       <c r="F29" t="s">
         <v>155</v>
       </c>
@@ -1223,6 +1244,9 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
+      <c r="C30" t="s">
+        <v>157</v>
+      </c>
       <c r="F30" t="s">
         <v>155</v>
       </c>
@@ -1236,6 +1260,9 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
+      <c r="C31" t="s">
+        <v>157</v>
+      </c>
       <c r="F31" t="s">
         <v>153</v>
       </c>
@@ -1288,6 +1315,9 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
+      <c r="C35" t="s">
+        <v>157</v>
+      </c>
       <c r="F35" t="s">
         <v>153</v>
       </c>
@@ -1301,6 +1331,9 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
+      <c r="C36" t="s">
+        <v>157</v>
+      </c>
       <c r="F36" t="s">
         <v>153</v>
       </c>
@@ -1314,6 +1347,9 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
+      <c r="C37" t="s">
+        <v>157</v>
+      </c>
       <c r="F37" t="s">
         <v>153</v>
       </c>
@@ -1327,6 +1363,9 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="C38" t="s">
+        <v>157</v>
+      </c>
       <c r="F38" t="s">
         <v>153</v>
       </c>
@@ -1340,6 +1379,9 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
       <c r="F39" t="s">
         <v>153</v>
       </c>
@@ -1353,6 +1395,9 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
+      <c r="C40" t="s">
+        <v>157</v>
+      </c>
       <c r="F40" t="s">
         <v>153</v>
       </c>
@@ -1366,6 +1411,9 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
+      <c r="C41" t="s">
+        <v>157</v>
+      </c>
       <c r="F41" t="s">
         <v>153</v>
       </c>
@@ -1379,6 +1427,9 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
+      <c r="C42" t="s">
+        <v>157</v>
+      </c>
       <c r="F42" t="s">
         <v>153</v>
       </c>
@@ -1392,6 +1443,9 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
+      <c r="C43" t="s">
+        <v>157</v>
+      </c>
       <c r="F43" t="s">
         <v>153</v>
       </c>
@@ -1444,6 +1498,9 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
+      <c r="C47" t="s">
+        <v>157</v>
+      </c>
       <c r="F47" t="s">
         <v>153</v>
       </c>
@@ -1457,6 +1514,9 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
+      <c r="C48" t="s">
+        <v>157</v>
+      </c>
       <c r="F48" t="s">
         <v>153</v>
       </c>
@@ -1633,7 +1693,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>158</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
@@ -1735,7 +1795,7 @@
         <v>78</v>
       </c>
       <c r="B74">
-        <f t="shared" ref="B74:B113" si="1">B73+1</f>
+        <f t="shared" ref="B74:B112" si="1">B73+1</f>
         <v>82</v>
       </c>
       <c r="M74" s="2"/>
@@ -1992,280 +2052,269 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B92">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M92" s="2"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M93" s="2"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F94" t="s">
+        <v>144</v>
       </c>
       <c r="M94" s="2"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F95" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M95" s="2"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F96" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M96" s="2"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F97" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="M97" s="2"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M98" s="2"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M99" s="2"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M100" s="2"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M101" s="2"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M102" s="2"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M103" s="2"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B104">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M104" s="2"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B105">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F105" t="s">
+        <v>149</v>
       </c>
       <c r="M105" s="2"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B106">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F106" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M106" s="2"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B107">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F107" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M107" s="2"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B108">
         <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="F108" t="s">
-        <v>148</v>
+        <v>24</v>
       </c>
       <c r="M108" s="2"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B109">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M109" s="2"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B110">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="F110" t="s">
+        <v>150</v>
       </c>
       <c r="M110" s="2"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B111">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F111" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M111" s="2"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B112">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F112" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M112" s="2"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>116</v>
-      </c>
-      <c r="B113">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="F113" t="s">
-        <v>152</v>
-      </c>
+    <row r="113" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M113" s="2"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M114" s="2"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M115" s="2"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M116" s="2"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M117" s="2"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M118" s="2"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M119" s="2"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M120" s="2"/>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M121" s="2"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M122" s="2"/>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="M123" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>